<commit_message>
Update 1911 - Michigan and Fixes
Updated all MI STARS and SIDS.
Pulled in new fixes.  Moved fixes.  From CIFP data.
</commit_message>
<xml_diff>
--- a/CIFPs/CIFP Schema Workbook.xlsx
+++ b/CIFPs/CIFP Schema Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/810620fc86a25db8/Documents/GitHub/ZOBFacilities/CIFPs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve_zxf9vd\OneDrive\Documents\GitHub\ZOBFacilities\CIFPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1187184-64D2-4D30-B664-9CE56448A665}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C1187184-64D2-4D30-B664-9CE56448A665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{222272D2-11A0-46BE-901E-F6E36D49A73A}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B524025B-1BDC-4D35-B6BA-643E4BE856DA}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B524025B-1BDC-4D35-B6BA-643E4BE856DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>Section Code</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>FIX ID END</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -334,85 +337,85 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,44 +431,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECFCFB0A-BA8F-4CD1-8FC1-0F28BE7CA3D2}" name="Table1" displayName="Table1" ref="A1:AC31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="26">
-  <autoFilter ref="A1:AC31" xr:uid="{17B89655-66B1-4FDD-BE88-20A22882113A}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECFCFB0A-BA8F-4CD1-8FC1-0F28BE7CA3D2}" name="Table1" displayName="Table1" ref="A1:AC32" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:AC32" xr:uid="{17B89655-66B1-4FDD-BE88-20A22882113A}"/>
   <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{91196D5D-1231-4CD6-8F7B-F085B0F554D4}" name="Section Code" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{C8AE10D7-40C5-4C8F-BF7E-BEE7B0B809EC}" name="Subsection" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{3B1FA408-78A9-41DE-ABB1-84E5B85B4E7F}" name="Name" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{14EBF888-ADDA-48FC-A917-29CA08EEE72D}" name="Keep" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{0F1EA90C-1944-4C98-BADE-B1A7D9842E41}" name="RECORD TYPE" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{EA0E32DE-C7B4-483C-BC2E-E6FE57FEB986}" name="CUSTOMER CODE START" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{5FD3DF76-CB32-49CE-85AE-5DAACF17C2D4}" name="CUSTOMER CODE END" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{C43A0889-33D7-4F2B-9CDA-75D2E6B3B6C8}" name="SECTION CODE2" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{77400821-0429-401F-8F45-3E5B2F47E575}" name="SUBSECTION CODE" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{9482C039-BB6F-4731-89DE-37A1EA32F280}" name="AIRPORT CODE START" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{E1814E65-69C5-404F-A397-4B03CED9350C}" name="AIRPORT CODE END" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{DBCFCBA9-9A06-443C-BF41-795493BB27EF}" name="ID START" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{488C0924-F913-44E0-A43A-994C5CAA9971}" name="ID END" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{08AB5F5F-4E51-49F9-B9D7-BE080F21F3EA}" name="FREQ START" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{A2E23E20-B4DC-4EDB-BB1D-E87719BAF9D2}" name="FREQ END" dataDxfId="15"/>
-    <tableColumn id="27" xr3:uid="{07416CF2-2229-4360-AB16-AB6298240E0C}" name="SEQ START" dataDxfId="2"/>
-    <tableColumn id="26" xr3:uid="{1ED1BEB7-1EAF-496D-9BE1-74C32CF64F22}" name="SEQ END" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{BE2D029A-D594-4F04-ACAF-336B89AA5F71}" name="FIX ID START" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{5E17CDC7-766B-4132-9880-BC8CDDA2162A}" name="FIX ID END" dataDxfId="0"/>
-    <tableColumn id="16" xr3:uid="{81C4E747-7520-4CA1-8D15-37EAF0E86780}" name="LAT START" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{64F27954-A8E3-4A54-8835-A0FB9E64A10D}" name="LAT LON" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{123B7442-2329-45D4-B24A-A5C5F5A3AFBA}" name="LON START" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{C552E1A3-D020-445F-8256-A493418E6B9A}" name="LON END" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{070AB524-9FFF-4179-98B3-DF4E8B26E469}" name="VOR NAME START" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{EAD9CDDC-9774-4D96-9BAA-9A14D38144D1}" name="VOR NAME END" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{7714314E-81AE-4260-AF4D-BB4C5ABC4E81}" name="FILE RECORD NO START" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{F28C4215-A041-4103-AD54-3051DAE06D3C}" name="FILE RECORD NO END" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{34BC9711-936F-45A7-A26E-800C6E5AA58B}" name="CYCLE DATE START" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{A798B6BC-9563-4D61-A17D-3EDC7F41537E}" name="CYCLE DATE END" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{91196D5D-1231-4CD6-8F7B-F085B0F554D4}" name="Section Code" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{C8AE10D7-40C5-4C8F-BF7E-BEE7B0B809EC}" name="Subsection" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{3B1FA408-78A9-41DE-ABB1-84E5B85B4E7F}" name="Name" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{14EBF888-ADDA-48FC-A917-29CA08EEE72D}" name="Keep" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{0F1EA90C-1944-4C98-BADE-B1A7D9842E41}" name="RECORD TYPE" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{EA0E32DE-C7B4-483C-BC2E-E6FE57FEB986}" name="CUSTOMER CODE START" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{5FD3DF76-CB32-49CE-85AE-5DAACF17C2D4}" name="CUSTOMER CODE END" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{C43A0889-33D7-4F2B-9CDA-75D2E6B3B6C8}" name="SECTION CODE2" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{77400821-0429-401F-8F45-3E5B2F47E575}" name="SUBSECTION CODE" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{9482C039-BB6F-4731-89DE-37A1EA32F280}" name="AIRPORT CODE START" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{E1814E65-69C5-404F-A397-4B03CED9350C}" name="AIRPORT CODE END" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{DBCFCBA9-9A06-443C-BF41-795493BB27EF}" name="ID START" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{488C0924-F913-44E0-A43A-994C5CAA9971}" name="ID END" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{08AB5F5F-4E51-49F9-B9D7-BE080F21F3EA}" name="FREQ START" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{A2E23E20-B4DC-4EDB-BB1D-E87719BAF9D2}" name="FREQ END" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{07416CF2-2229-4360-AB16-AB6298240E0C}" name="SEQ START" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{1ED1BEB7-1EAF-496D-9BE1-74C32CF64F22}" name="SEQ END" dataDxfId="12"/>
+    <tableColumn id="28" xr3:uid="{BE2D029A-D594-4F04-ACAF-336B89AA5F71}" name="FIX ID START" dataDxfId="11"/>
+    <tableColumn id="29" xr3:uid="{5E17CDC7-766B-4132-9880-BC8CDDA2162A}" name="FIX ID END" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{81C4E747-7520-4CA1-8D15-37EAF0E86780}" name="LAT START" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{64F27954-A8E3-4A54-8835-A0FB9E64A10D}" name="LAT LON" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{123B7442-2329-45D4-B24A-A5C5F5A3AFBA}" name="LON START" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{C552E1A3-D020-445F-8256-A493418E6B9A}" name="LON END" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{070AB524-9FFF-4179-98B3-DF4E8B26E469}" name="VOR NAME START" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{EAD9CDDC-9774-4D96-9BAA-9A14D38144D1}" name="VOR NAME END" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{7714314E-81AE-4260-AF4D-BB4C5ABC4E81}" name="FILE RECORD NO START" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{F28C4215-A041-4103-AD54-3051DAE06D3C}" name="FILE RECORD NO END" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{34BC9711-936F-45A7-A26E-800C6E5AA58B}" name="CYCLE DATE START" dataDxfId="1"/>
+    <tableColumn id="25" xr3:uid="{A798B6BC-9563-4D61-A17D-3EDC7F41537E}" name="CYCLE DATE END" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,13 +765,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033C8353-F4C2-45C6-B241-D4333130586D}">
-  <dimension ref="A1:AC31"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +883,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1154,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1190,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1298,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1337,7 +1334,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +1373,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1415,7 +1412,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1458,36 +1455,19 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>4</v>
-      </c>
-      <c r="H13" s="1">
-        <v>5</v>
-      </c>
-      <c r="I13" s="1">
-        <v>6</v>
-      </c>
-      <c r="J13" s="1">
-        <v>7</v>
-      </c>
-      <c r="K13" s="1">
-        <v>10</v>
-      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1500,45 +1480,47 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="1">
-        <v>94</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>123</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>124</v>
-      </c>
-      <c r="AA13" s="1">
-        <v>128</v>
-      </c>
-      <c r="AB13" s="1">
-        <v>129</v>
-      </c>
-      <c r="AC13" s="1">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1">
+        <v>10</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1551,95 +1533,73 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="1">
+        <v>94</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>123</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>124</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>128</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>129</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
-      <c r="H15" s="1">
-        <v>5</v>
-      </c>
-      <c r="I15" s="1">
-        <v>6</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1">
-        <v>14</v>
-      </c>
-      <c r="M15" s="1">
-        <v>18</v>
-      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1">
-        <v>33</v>
-      </c>
-      <c r="U15" s="1">
-        <v>41</v>
-      </c>
-      <c r="V15" s="1">
-        <v>42</v>
-      </c>
-      <c r="W15" s="1">
-        <v>51</v>
-      </c>
-      <c r="X15" s="1">
-        <v>99</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>123</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>124</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>128</v>
-      </c>
-      <c r="AB15" s="1">
-        <v>129</v>
-      </c>
-      <c r="AC15" s="1">
-        <v>132</v>
-      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="b">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1653,41 +1613,41 @@
       <c r="H16" s="1">
         <v>5</v>
       </c>
-      <c r="I16" s="4">
-        <v>13</v>
-      </c>
-      <c r="J16" s="1">
-        <v>7</v>
-      </c>
-      <c r="K16" s="1">
-        <v>10</v>
-      </c>
+      <c r="I16" s="1">
+        <v>6</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
       <c r="L16" s="1">
         <v>14</v>
       </c>
       <c r="M16" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1">
-        <v>27</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>29</v>
-      </c>
-      <c r="R16" s="1">
-        <v>30</v>
-      </c>
-      <c r="S16" s="1">
-        <v>34</v>
-      </c>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1">
+        <v>33</v>
+      </c>
+      <c r="U16" s="1">
+        <v>41</v>
+      </c>
+      <c r="V16" s="1">
+        <v>42</v>
+      </c>
+      <c r="W16" s="1">
+        <v>51</v>
+      </c>
+      <c r="X16" s="1">
+        <v>99</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>123</v>
+      </c>
       <c r="Z16" s="1">
         <v>124</v>
       </c>
@@ -1706,10 +1666,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="b">
         <v>1</v>
@@ -1774,51 +1734,88 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>13</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7</v>
+      </c>
+      <c r="K18" s="1">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
+        <v>14</v>
+      </c>
+      <c r="M18" s="1">
+        <v>19</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="P18" s="1">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>29</v>
+      </c>
+      <c r="R18" s="1">
+        <v>30</v>
+      </c>
+      <c r="S18" s="1">
+        <v>34</v>
+      </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Z18" s="1">
+        <v>124</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>128</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>129</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1846,15 +1843,15 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1882,18 +1879,15 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="1" t="b">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1921,15 +1915,18 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1957,18 +1954,15 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1" t="b">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1996,15 +1990,18 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
     </row>
-    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2032,18 +2029,15 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="1" t="b">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2071,15 +2065,15 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
     </row>
-    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="b">
         <v>0</v>
@@ -2110,15 +2104,15 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>0</v>
@@ -2149,15 +2143,15 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
-    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1" t="b">
         <v>0</v>
@@ -2188,15 +2182,15 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D29" s="1" t="b">
         <v>0</v>
@@ -2227,15 +2221,15 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1" t="b">
         <v>0</v>
@@ -2266,15 +2260,15 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
@@ -2305,6 +2299,45 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>